<commit_message>
Checking in changes in BR
</commit_message>
<xml_diff>
--- a/seeddata-bsdf/99-exceldmd/Governance App Model.xlsx
+++ b/seeddata-bsdf/99-exceldmd/Governance App Model.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilbhatia/github/Beiersdorf/seeddata-bsdf/99-exceldmd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\advellencesolutionag\Beiersdorf\seeddata-bsdf\99-exceldmd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="23540" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="23535" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="REF DATA" sheetId="10" r:id="rId1"/>
@@ -38,14 +38,14 @@
     <definedName name="Z_F59B42B5_12A6_408C_8984_297F5E3274B0_.wvu.FilterData" localSheetId="3" hidden="1">'BUSINESS RULES'!$A$1:$I$1</definedName>
     <definedName name="Z_F59B42B5_12A6_408C_8984_297F5E3274B0_.wvu.FilterData" localSheetId="7" hidden="1">'SYSTEM MESSAGES'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
-    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="126">
   <si>
     <t>ACTION</t>
   </si>
@@ -321,21 +321,9 @@
     <t>Send PV For Entity For GraphProcessing</t>
   </si>
   <si>
-    <t>IIF[ValidateEmptyAttributes["aid"],AddAttributeError["Req001", "", "aid"],AddAttributeInformation["SYS001", "", "aid"]] AND IIF[ValidateEmptyAttributes["aidentifier"],AddAttributeError["Req001", "", "aidentifier"],AddAttributeInformation["SYS001", "", "aidentifier"]] AND IIF[ValidateEmptyAttributes["adescription"],AddAttributeError["Req001", "", "adescription"],AddAttributeInformation["SYS001", "", "adescription"]]</t>
-  </si>
-  <si>
     <t>IIF[IsEntityInWorkflow["newNartSetup"] ,true,InvokeWorkflow["newNartSetup"]]</t>
   </si>
   <si>
-    <t>IIF[IsEntityInWorkflow["newNartSetup"],AddAttributeInformation["SYS001", "", "unknown"],AddAttributeError["Req001", "", "unknown"]]</t>
-  </si>
-  <si>
-    <t>IIF[HaveAnyAttributesChanged["primaryimage","alternateimages"],SendEntityForGraphProcessing["enart_hasimages_image"],false]</t>
-  </si>
-  <si>
-    <t>IIF[HaveAnyAttributesChanged["_ALL"],SendEntityForGraphProcessing["eproductversion_ischildof_enart"],false]</t>
-  </si>
-  <si>
     <t>Business Required attributes need to be completed</t>
   </si>
   <si>
@@ -396,18 +384,9 @@
     <t>setApprovalFlagForNart</t>
   </si>
   <si>
-    <t>IIF[HaveAnyAttributesChanged["productversionapproved"] AND IsEntityInWorkflow["newLBUNartSetup"]=false,InvokeWorkflow["newLBUNartSetup"],false]</t>
-  </si>
-  <si>
     <t>processGraphProcessToCopyPVApproval</t>
   </si>
   <si>
-    <t>IIF[ValidateEmptyAttributes["productversionapproved"],SetAttributeValue["_DEFAULT","_DEFAULT","productversionapproved",true] ,false]</t>
-  </si>
-  <si>
-    <t>IIF[HaveAnyAttributesChanged["productversionapproved"],SendEntityForGraphProcessing["eproductversion_ischildof_enart","newPVSetup","gbuMediaEnrichment","Done"],false]</t>
-  </si>
-  <si>
     <t>Invoke Nart Workflow on PV Approval</t>
   </si>
   <si>
@@ -418,12 +397,48 @@
   </si>
   <si>
     <t>update</t>
+  </si>
+  <si>
+    <t>Any</t>
+  </si>
+  <si>
+    <t>populateDescription</t>
+  </si>
+  <si>
+    <t>IIF[GetAttributeValue["_DEFAULT","_DEFAULT","abeautyritual"] ="test",SetAttributeValue["_DEFAULT","_DEFAULT","abacksidetext","Business rule fired"],false]</t>
+  </si>
+  <si>
+    <t>auto populate itemtype</t>
+  </si>
+  <si>
+    <t>This is the step where Business will approve the SKU(s) submitted by the vendor and approved by the Buyer.</t>
+  </si>
+  <si>
+    <t>IIF[HaveAnyAttributesChanged["","","productversionapproved"],SendEntityForGraphProcessing["eproductversion_ischildof_enart","newPVSetup","gbuMediaEnrichment","Done"],false]</t>
+  </si>
+  <si>
+    <t>IIF[HaveAnyAttributesChanged["","","primaryimage","alternateimages"],SendEntityForGraphProcessing["enart_hasimages_image"],false]</t>
+  </si>
+  <si>
+    <t>IIF[HaveAnyAttributesChanged["","","_ALL"],SendEntityForGraphProcessing["eproductversion_ischildof_enart"],false]</t>
+  </si>
+  <si>
+    <t>IIF[HaveAnyAttributesChanged["","","productversionapproved"] AND IsEntityInWorkflow["newLBUNartSetup"]=false,InvokeWorkflow["newLBUNartSetup"],false]</t>
+  </si>
+  <si>
+    <t>IIF[IsEntityInWorkflow["newNartSetup"],AddAttributeInformation["_DEFAULT","_DEFAULT","SYS001", "", "unknown"],AddAttributeError["_DEFAULT","_DEFAULT","Req001", "", "unknown"]]</t>
+  </si>
+  <si>
+    <t>IIF[ValidateEmptyAttributes["_DEFAULT","_DEFAULT","productversionapproved"],SetAttributeValue["_DEFAULT","_DEFAULT","productversionapproved",true] ,false]</t>
+  </si>
+  <si>
+    <t>IIF[ValidateEmptyAttributes["_DEFAULT","_DEFAULT","adescription"],AddAttributeError["_DEFAULT","_DEFAULT","Req001", "", "adescription"],AddAttributeInformation["_DEFAULT","_DEFAULT","SYS001", "", "adescription"]] AND IIF[ValidateEmptyAttributes["_DEFAULT","_DEFAULT","aid"],AddAttributeError["_DEFAULT","_DEFAULT","Req001", "", "aid"],AddAttributeInformation["_DEFAULT","_DEFAULT","SYS001", "", "aid"]] AND IIF[ValidateEmptyAttributes["_DEFAULT","_DEFAULT","aidentifier"],AddAttributeError["_DEFAULT","_DEFAULT","Req001", "", "aidentifier"],AddAttributeInformation["_DEFAULT","_DEFAULT","SYS001", "", "aidentifier"]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
   </numFmts>
@@ -1285,16 +1300,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1357,14 +1372,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="104" bestFit="1" customWidth="1"/>
@@ -1400,12 +1415,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
+      <selection activeCell="B34" sqref="B34"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
       <selection activeCell="A5" sqref="A5"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
-      <selection activeCell="B34" sqref="B34"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -1415,23 +1430,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A4:F11"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
@@ -1448,7 +1463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
@@ -1465,7 +1480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -1482,7 +1497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
@@ -1499,7 +1514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
         <v>7</v>
@@ -1514,7 +1529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15" t="s">
         <v>9</v>
@@ -1529,7 +1544,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="14" t="s">
         <v>8</v>
@@ -1538,7 +1553,7 @@
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="17" t="s">
         <v>20</v>
@@ -1549,11 +1564,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -1565,28 +1580,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I10"/>
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="7.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="133.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="83.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="133.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="83.375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1615,7 +1630,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="242.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>76</v>
       </c>
@@ -1632,13 +1647,13 @@
         <v>35</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
         <v>74</v>
       </c>
@@ -1655,14 +1670,14 @@
         <v>35</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H3" s="25" t="s">
         <v>71</v>
       </c>
       <c r="I3" s="25"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
         <v>82</v>
       </c>
@@ -1679,13 +1694,13 @@
         <v>35</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="H4" s="25" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
         <v>84</v>
       </c>
@@ -1702,13 +1717,13 @@
         <v>35</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="H5" s="25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
         <v>86</v>
       </c>
@@ -1725,15 +1740,15 @@
         <v>35</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>42</v>
@@ -1748,15 +1763,15 @@
         <v>35</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
         <v>42</v>
@@ -1771,15 +1786,15 @@
         <v>35</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
         <v>42</v>
@@ -1794,15 +1809,15 @@
         <v>35</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
         <v>42</v>
@@ -1817,23 +1832,49 @@
         <v>35</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>119</v>
+      <c r="H11" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I3"/>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -1855,48 +1896,48 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AC233"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="87" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="7.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="64.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.875" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.125" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="18" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1931,7 +1972,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="25"/>
       <c r="B2" s="25" t="s">
         <v>76</v>
@@ -1949,20 +1990,20 @@
         <v>76</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
       <c r="B3" s="25" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>81</v>
@@ -1977,109 +2018,109 @@
         <v>82</v>
       </c>
       <c r="G3" s="25" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H3" s="25"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="25"/>
       <c r="B4" s="20"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="25"/>
       <c r="B5" s="20"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="20"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
       <c r="B7" s="20"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
       <c r="B8" s="20"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
       <c r="B9" s="20"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="20"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="25"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="25"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="25"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="25"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="25"/>
       <c r="G15" s="25"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="25"/>
       <c r="G16" s="25"/>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="25"/>
       <c r="G17" s="25"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="25"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="25"/>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="25"/>
       <c r="B32" s="22"/>
       <c r="C32" s="22"/>
@@ -2102,446 +2143,446 @@
       <c r="Z32" s="22"/>
       <c r="AC32" s="22"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="25"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="25"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="25"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="25"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="25"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="25"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="25"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="25"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="25"/>
       <c r="F42" s="22"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="25"/>
       <c r="F43" s="22"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="25"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="25"/>
       <c r="F45" s="22"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="25"/>
       <c r="F46" s="22"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="25"/>
       <c r="F47" s="22"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="F48" s="22"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="25"/>
       <c r="F49" s="22"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="25"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="25"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="25"/>
       <c r="F52" s="22"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="25"/>
       <c r="F53" s="22"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="25"/>
       <c r="F54" s="22"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="25"/>
       <c r="F55" s="22"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="25"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="25"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="25"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="25"/>
       <c r="F59" s="22"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="25"/>
       <c r="F60" s="22"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="25"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="25"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="25"/>
       <c r="F63" s="22"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="25"/>
       <c r="F64" s="22"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="25"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="25"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="25"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="25"/>
       <c r="F68" s="22"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="25"/>
       <c r="F69" s="22"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="25"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="25"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="25"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="25"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="25"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="25"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="25"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="25"/>
       <c r="F77" s="22"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="25"/>
       <c r="F78" s="22"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="25"/>
       <c r="F79" s="22"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="25"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="25"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="25"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="25"/>
       <c r="K83" s="25"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="25"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="25"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="25"/>
       <c r="F86" s="22"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="25"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="25"/>
       <c r="F88" s="22"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="25"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="25"/>
       <c r="F90" s="22"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="25"/>
       <c r="F91" s="22"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="25"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="25"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="25"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="25"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="25"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="25"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="25"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="25"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="25"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="25"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="25"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="25"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="25"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="25"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="25"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="25"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="25"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="25"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="25"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="25"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="25"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="25"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="25"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="25"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="25"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="25"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="25"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="25"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="25"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="25"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="25"/>
       <c r="B122" s="20"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="25"/>
       <c r="B123" s="20"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="25"/>
       <c r="B124" s="20"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="25"/>
       <c r="B125" s="20"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="25"/>
       <c r="B126" s="20"/>
       <c r="F126" s="21"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="25"/>
       <c r="B127" s="20"/>
       <c r="F127" s="21"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="25"/>
       <c r="B128" s="20"/>
       <c r="F128" s="21"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="25"/>
       <c r="B129" s="20"/>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="25"/>
       <c r="B130" s="20"/>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="25"/>
       <c r="B131" s="20"/>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="25"/>
       <c r="B132" s="20"/>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="25"/>
       <c r="B133" s="20"/>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="25"/>
       <c r="B134" s="20"/>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="25"/>
       <c r="B135" s="20"/>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="25"/>
       <c r="B136" s="20"/>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="25"/>
       <c r="B137" s="21"/>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="25"/>
       <c r="B138" s="20"/>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="25"/>
       <c r="B139" s="20"/>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="25"/>
       <c r="B140" s="20"/>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="25"/>
       <c r="B141" s="20"/>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="25"/>
       <c r="B142" s="20"/>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="25"/>
       <c r="B143" s="20"/>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="25"/>
       <c r="B144" s="20"/>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A145" s="25"/>
       <c r="B145" s="20"/>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A146" s="25"/>
       <c r="B146" s="20"/>
     </row>
-    <row r="147" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A147" s="25"/>
       <c r="B147" s="20"/>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A148" s="25"/>
       <c r="B148" s="20"/>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A149" s="25"/>
       <c r="B149" s="20"/>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A150" s="25"/>
       <c r="B150" s="20"/>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A151" s="25"/>
       <c r="B151" s="20"/>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A152" s="25"/>
       <c r="B152" s="20"/>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A153" s="25"/>
       <c r="B153" s="20"/>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A154" s="25"/>
       <c r="B154" s="21"/>
     </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A155" s="25"/>
       <c r="B155" s="21"/>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A156" s="25"/>
       <c r="B156" s="21"/>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A157" s="25"/>
       <c r="I157" s="19"/>
       <c r="J157" s="19"/>
@@ -2550,134 +2591,134 @@
       <c r="AB157" s="19"/>
       <c r="AC157" s="19"/>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A158" s="25"/>
       <c r="B158" s="20"/>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A159" s="25"/>
       <c r="B159" s="20"/>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A160" s="25"/>
       <c r="B160" s="20"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="25"/>
       <c r="B161" s="20"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="25"/>
       <c r="B162" s="20"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="25"/>
       <c r="B163" s="20"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="25"/>
       <c r="B164" s="20"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="25"/>
       <c r="B165" s="20"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="25"/>
       <c r="B166" s="20"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="25"/>
       <c r="B167" s="20"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="25"/>
       <c r="B168" s="20"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="25"/>
       <c r="B169" s="20"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="25"/>
       <c r="B170" s="20"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="25"/>
       <c r="B171" s="20"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="25"/>
       <c r="B172" s="20"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="25"/>
       <c r="B173" s="20"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="25"/>
       <c r="B174" s="20"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="25"/>
       <c r="B175" s="20"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="25"/>
       <c r="B176" s="20"/>
     </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A177" s="25"/>
       <c r="B177" s="20"/>
     </row>
-    <row r="178" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A178" s="25"/>
       <c r="B178" s="20"/>
     </row>
-    <row r="179" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A179" s="25"/>
       <c r="B179" s="20"/>
     </row>
-    <row r="180" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A180" s="25"/>
       <c r="B180" s="20"/>
     </row>
-    <row r="181" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A181" s="25"/>
       <c r="B181" s="20"/>
     </row>
-    <row r="182" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A182" s="25"/>
       <c r="B182" s="20"/>
     </row>
-    <row r="183" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A183" s="25"/>
       <c r="B183" s="20"/>
     </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A184" s="25"/>
       <c r="B184" s="20"/>
     </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A185" s="25"/>
       <c r="B185" s="20"/>
     </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A186" s="25"/>
       <c r="B186" s="20"/>
     </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A187" s="25"/>
       <c r="B187" s="20"/>
     </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A188" s="25"/>
       <c r="B188" s="20"/>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A189" s="25"/>
     </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A190" s="25"/>
       <c r="B190" s="21"/>
       <c r="I190" s="19"/>
@@ -2685,7 +2726,7 @@
       <c r="K190" s="19"/>
       <c r="AC190" s="19"/>
     </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A191" s="25"/>
       <c r="B191" s="21"/>
       <c r="I191" s="19"/>
@@ -2695,7 +2736,7 @@
       <c r="AB191" s="19"/>
       <c r="AC191" s="19"/>
     </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A192" s="25"/>
       <c r="B192" s="21"/>
       <c r="I192" s="19"/>
@@ -2704,7 +2745,7 @@
       <c r="AA192" s="19"/>
       <c r="AC192" s="19"/>
     </row>
-    <row r="193" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A193" s="25"/>
       <c r="B193" s="21"/>
       <c r="C193" s="20"/>
@@ -2715,18 +2756,18 @@
       <c r="AB193" s="19"/>
       <c r="AC193" s="19"/>
     </row>
-    <row r="194" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A194" s="25"/>
       <c r="B194" s="21"/>
       <c r="C194" s="20"/>
       <c r="F194" s="20"/>
     </row>
-    <row r="195" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A195" s="25"/>
       <c r="B195" s="21"/>
       <c r="C195" s="20"/>
     </row>
-    <row r="196" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A196" s="25"/>
       <c r="B196" s="24"/>
       <c r="C196" s="20"/>
@@ -2737,149 +2778,149 @@
       <c r="AB196" s="23"/>
       <c r="AC196" s="23"/>
     </row>
-    <row r="197" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A197" s="25"/>
       <c r="B197" s="21"/>
       <c r="C197" s="20"/>
       <c r="F197" s="20"/>
     </row>
-    <row r="198" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A198" s="25"/>
       <c r="B198" s="21"/>
       <c r="C198" s="20"/>
       <c r="F198" s="20"/>
     </row>
-    <row r="199" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A199" s="25"/>
       <c r="B199" s="21"/>
     </row>
-    <row r="200" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A200" s="25"/>
       <c r="B200" s="21"/>
     </row>
-    <row r="201" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A201" s="25"/>
       <c r="B201" s="21"/>
       <c r="K201" s="25"/>
     </row>
-    <row r="202" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A202" s="25"/>
       <c r="B202" s="21"/>
       <c r="K202" s="25"/>
     </row>
-    <row r="203" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A203" s="25"/>
       <c r="B203" s="21"/>
     </row>
-    <row r="204" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A204" s="25"/>
       <c r="B204" s="21"/>
     </row>
-    <row r="205" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A205" s="25"/>
       <c r="B205" s="21"/>
       <c r="F205" s="22"/>
     </row>
-    <row r="206" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A206" s="25"/>
       <c r="B206" s="21"/>
       <c r="F206" s="22"/>
     </row>
-    <row r="207" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A207" s="25"/>
       <c r="B207" s="21"/>
       <c r="F207" s="22"/>
     </row>
-    <row r="208" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A208" s="25"/>
       <c r="B208" s="21"/>
       <c r="F208" s="22"/>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="25"/>
       <c r="B209" s="21"/>
       <c r="F209" s="22"/>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="25"/>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="25"/>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="25"/>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="25"/>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="25"/>
       <c r="B214" s="21"/>
     </row>
-    <row r="215" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H215" s="6"/>
     </row>
-    <row r="216" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H216" s="6"/>
     </row>
-    <row r="217" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H217" s="6"/>
     </row>
-    <row r="218" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H218" s="6"/>
     </row>
-    <row r="219" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H219" s="6"/>
     </row>
-    <row r="220" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H220" s="6"/>
     </row>
-    <row r="221" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H221" s="6"/>
     </row>
-    <row r="222" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H222" s="6"/>
     </row>
-    <row r="223" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H223" s="6"/>
     </row>
-    <row r="224" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H224" s="6"/>
     </row>
-    <row r="225" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H225" s="6"/>
     </row>
-    <row r="226" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H226" s="6"/>
     </row>
-    <row r="227" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H227" s="6"/>
     </row>
-    <row r="228" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H228" s="6"/>
     </row>
-    <row r="229" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H229" s="6"/>
     </row>
-    <row r="230" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="H230" s="6"/>
     </row>
-    <row r="231" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B231" s="21"/>
       <c r="H231" s="6"/>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="25"/>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:K2"/>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -2887,9 +2928,9 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:AE347"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -2940,31 +2981,31 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:L9"/>
+  <sheetPr codeName="Sheet6"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView zoomScale="165" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.33203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" style="25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.875" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.375" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.875" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.125" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3002,9 +3043,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C2" s="25" t="s">
         <v>81</v>
@@ -3029,12 +3070,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>10</v>
@@ -3053,9 +3094,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C4" s="25" t="s">
         <v>81</v>
@@ -3067,7 +3108,7 @@
         <v>35</v>
       </c>
       <c r="F4" s="25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G4" s="22"/>
       <c r="H4" s="22" t="s">
@@ -3081,9 +3122,9 @@
       </c>
       <c r="L4" s="25"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>81</v>
@@ -3095,7 +3136,7 @@
         <v>35</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G5" s="22"/>
       <c r="J5" s="25">
@@ -3105,9 +3146,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C6" s="25" t="s">
         <v>81</v>
@@ -3119,14 +3160,14 @@
         <v>35</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I6" s="25" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J6" s="25">
         <v>1</v>
@@ -3135,9 +3176,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C7" s="25" t="s">
         <v>81</v>
@@ -3149,14 +3190,14 @@
         <v>35</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="22" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="I7" s="25" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J7" s="25">
         <v>10</v>
@@ -3165,9 +3206,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
         <v>81</v>
@@ -3182,7 +3223,7 @@
         <v>76</v>
       </c>
       <c r="I8" s="25" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J8" s="25">
         <v>1</v>
@@ -3191,9 +3232,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C9" s="25" t="s">
         <v>81</v>
@@ -3205,10 +3246,10 @@
         <v>35</v>
       </c>
       <c r="G9" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="25" t="s">
         <v>96</v>
-      </c>
-      <c r="I9" s="25" t="s">
-        <v>100</v>
       </c>
       <c r="J9" s="25">
         <v>2</v>
@@ -3216,18 +3257,72 @@
       <c r="K9" s="25" t="s">
         <v>10</v>
       </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="J10" s="25">
+        <v>1</v>
+      </c>
+      <c r="K10" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="25"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="J11" s="25">
+        <v>1</v>
+      </c>
+      <c r="K11" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L4"/>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -3244,7 +3339,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
@@ -3252,22 +3347,22 @@
       <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.125" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.875" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="33.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3302,7 +3397,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="25" t="s">
         <v>80</v>
       </c>
@@ -3325,18 +3420,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>55</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H3" t="s">
         <v>73</v>
@@ -3348,18 +3443,18 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
         <v>55</v>
       </c>
       <c r="F4" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="G4" t="s">
         <v>99</v>
-      </c>
-      <c r="G4" t="s">
-        <v>103</v>
       </c>
       <c r="H4" t="s">
         <v>79</v>
@@ -3368,7 +3463,7 @@
         <v>79</v>
       </c>
       <c r="J4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3377,12 +3472,12 @@
     <sortCondition ref="B2"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3395,26 +3490,26 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -3442,6 +3537,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AA594"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="130" filter="1" showAutoFilter="1" hiddenRows="1">
       <selection activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3452,12 +3553,6 @@
           </filters>
         </filterColumn>
       </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AA594"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="B1 D1 F1 H1">
@@ -3480,15 +3575,53 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-24</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">
-      <Url>https://jcp.sharepoint.com/sites/SPOProjects/JCPDotcomPortfolio/AssortmentExpansion/_layouts/15/DocIdRedir.aspx?ID=Z7QZ4QWJDNQ7-73874190-24</Url>
-      <Description>Z7QZ4QWJDNQ7-73874190-24</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3670,53 +3803,15 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-24</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">
+      <Url>https://jcp.sharepoint.com/sites/SPOProjects/JCPDotcomPortfolio/AssortmentExpansion/_layouts/15/DocIdRedir.aspx?ID=Z7QZ4QWJDNQ7-73874190-24</Url>
+      <Description>Z7QZ4QWJDNQ7-73874190-24</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3728,18 +3823,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E9ADEF4-6C25-4BA4-9EDB-E28F722B8411}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58437D0-211E-4689-9BB7-1D7150BF8997}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="2e2046eb-f52d-433a-aad8-97c651e3992c"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3764,9 +3850,18 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58437D0-211E-4689-9BB7-1D7150BF8997}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E9ADEF4-6C25-4BA4-9EDB-E28F722B8411}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="2e2046eb-f52d-433a-aad8-97c651e3992c"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed the grapha processing and updated the business rule context definition.
</commit_message>
<xml_diff>
--- a/seeddata-bsdf/99-exceldmd/Governance App Model.xlsx
+++ b/seeddata-bsdf/99-exceldmd/Governance App Model.xlsx
@@ -38,7 +38,7 @@
     <definedName name="Z_F59B42B5_12A6_408C_8984_297F5E3274B0_.wvu.FilterData" localSheetId="3" hidden="1">'BUSINESS RULES'!$A$1:$I$1</definedName>
     <definedName name="Z_F59B42B5_12A6_408C_8984_297F5E3274B0_.wvu.FilterData" localSheetId="7" hidden="1">'SYSTEM MESSAGES'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <customWorkbookViews>
     <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="126">
   <si>
     <t>ACTION</t>
   </si>
@@ -414,9 +414,6 @@
     <t>This is the step where Business will approve the SKU(s) submitted by the vendor and approved by the Buyer.</t>
   </si>
   <si>
-    <t>IIF[HaveAnyAttributesChanged["","","productversionapproved"],SendEntityForGraphProcessing["eproductversion_ischildof_enart","newPVSetup","gbuMediaEnrichment","Done"],false]</t>
-  </si>
-  <si>
     <t>IIF[HaveAnyAttributesChanged["","","primaryimage","alternateimages"],SendEntityForGraphProcessing["enart_hasimages_image"],false]</t>
   </si>
   <si>
@@ -433,6 +430,9 @@
   </si>
   <si>
     <t>IIF[ValidateEmptyAttributes["_DEFAULT","_DEFAULT","adescription"],AddAttributeError["_DEFAULT","_DEFAULT","Req001", "", "adescription"],AddAttributeInformation["_DEFAULT","_DEFAULT","SYS001", "", "adescription"]] AND IIF[ValidateEmptyAttributes["_DEFAULT","_DEFAULT","aid"],AddAttributeError["_DEFAULT","_DEFAULT","Req001", "", "aid"],AddAttributeInformation["_DEFAULT","_DEFAULT","SYS001", "", "aid"]] AND IIF[ValidateEmptyAttributes["_DEFAULT","_DEFAULT","aidentifier"],AddAttributeError["_DEFAULT","_DEFAULT","Req001", "", "aidentifier"],AddAttributeInformation["_DEFAULT","_DEFAULT","SYS001", "", "aidentifier"]]</t>
+  </si>
+  <si>
+    <t>SendEntityForGraphProcessing["eproductversion_ischildof_enart","newPVSetup","gbuMediaEnrichment","Done"]</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1446,7 @@
     <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
       <c r="B8" s="13" t="s">
         <v>7</v>
@@ -1529,7 +1529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="15" t="s">
         <v>9</v>
@@ -1583,9 +1583,9 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1647,7 +1647,7 @@
         <v>35</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>75</v>
@@ -1694,7 +1694,7 @@
         <v>35</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H4" s="25" t="s">
         <v>83</v>
@@ -1717,7 +1717,7 @@
         <v>35</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H5" s="25" t="s">
         <v>85</v>
@@ -1740,7 +1740,7 @@
         <v>35</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H6" s="25" t="s">
         <v>87</v>
@@ -1786,7 +1786,7 @@
         <v>35</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>110</v>
@@ -1809,7 +1809,7 @@
         <v>35</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>111</v>
@@ -1832,7 +1832,7 @@
         <v>35</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>112</v>
@@ -1901,7 +1901,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2986,7 +2986,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3163,9 +3163,7 @@
         <v>108</v>
       </c>
       <c r="G6" s="22"/>
-      <c r="H6" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="H6" s="22"/>
       <c r="I6" s="25" t="s">
         <v>98</v>
       </c>
@@ -3193,9 +3191,7 @@
         <v>109</v>
       </c>
       <c r="G7" s="22"/>
-      <c r="H7" s="22" t="s">
-        <v>113</v>
-      </c>
+      <c r="H7" s="22"/>
       <c r="I7" s="25" t="s">
         <v>98</v>
       </c>
@@ -3362,7 +3358,7 @@
     <col min="11" max="11" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.95" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>